<commit_message>
System Setup4: sydefault, Inv comcod
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/CRUD-Feature Category.xlsx
+++ b/templates/AutomationOrg/CRUD-Feature Category.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkakade\Provar\Workspace\System Setup\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64788ECD-D211-4F7C-8DAC-A1B8FEC60AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F448D3D-5458-480B-8E18-AA78BDAF253D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3372" windowWidth="15912" windowHeight="8964" activeTab="1" xr2:uid="{2BFEB1D0-4BA7-4099-BD39-D94593123DD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2BFEB1D0-4BA7-4099-BD39-D94593123DD3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Create_Feature Category_x0009_" sheetId="1" r:id="rId1"/>
-    <sheet name="Edit_Feature Category_x0009_" sheetId="2" r:id="rId2"/>
+    <sheet name="Create_Feature Category" sheetId="3" r:id="rId1"/>
+    <sheet name="Edit_Feature Category" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,36 +36,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t xml:space="preserve">Feature Category	</t>
   </si>
   <si>
-    <t xml:space="preserve">Category Description	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Selection Sequence	</t>
-  </si>
-  <si>
     <t>PK_FC1</t>
   </si>
   <si>
     <t xml:space="preserve">Feature Category - Update	</t>
   </si>
   <si>
-    <t>Feature ID</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
-    <t>Feature Description</t>
-  </si>
-  <si>
     <t>Color- Red</t>
   </si>
   <si>
-    <t>Feature Category</t>
+    <t>FeatureCategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CategoryDescription	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DefaultSelectionSequence	</t>
+  </si>
+  <si>
+    <t>FeatureID</t>
+  </si>
+  <si>
+    <t>FeatureDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FeatureCategory	</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E3C161-DE6A-44B9-AA26-C2FC13E3FB40}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10039AF2-66CC-40B0-9DAC-B47C603600AC}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -424,33 +427,27 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -459,10 +456,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -471,36 +468,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C4E7B6-22B2-4403-BFBD-38290CFA728B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C10730-7E85-42C1-90FD-30995AE34D99}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>10</v>

</xml_diff>